<commit_message>
dans les psy ano aussi
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RPSA ANO 12.xlsx
+++ b/formats/excel/Formats RPSA ANO 12.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Github/formats_pmeasyr/formats/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="10800"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="27340" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -240,9 +253,6 @@
     <t>NOSEJ</t>
   </si>
   <si>
-    <t>NOSEJPSY</t>
-  </si>
-  <si>
     <t>DTENT</t>
   </si>
   <si>
@@ -364,6 +374,9 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>NOSEQSEJ</t>
   </si>
 </sst>
 </file>
@@ -418,7 +431,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -456,14 +469,14 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -493,12 +506,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -528,7 +541,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -704,17 +717,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="105.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="105.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -734,7 +747,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -751,10 +764,10 @@
         <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -771,10 +784,10 @@
         <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -791,10 +804,10 @@
         <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -811,10 +824,10 @@
         <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -831,10 +844,10 @@
         <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -851,10 +864,10 @@
         <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -871,10 +884,10 @@
         <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -891,10 +904,10 @@
         <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -911,10 +924,10 @@
         <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -931,10 +944,10 @@
         <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -951,10 +964,10 @@
         <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -971,10 +984,10 @@
         <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -991,10 +1004,10 @@
         <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1011,10 +1024,10 @@
         <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1031,10 +1044,10 @@
         <v>73</v>
       </c>
       <c r="F16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1048,13 +1061,13 @@
         <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1068,13 +1081,13 @@
         <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1088,13 +1101,13 @@
         <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1108,13 +1121,13 @@
         <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1128,13 +1141,13 @@
         <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1148,13 +1161,13 @@
         <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1168,13 +1181,13 @@
         <v>85</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1188,13 +1201,13 @@
         <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1208,13 +1221,13 @@
         <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1228,13 +1241,13 @@
         <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1248,13 +1261,13 @@
         <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1268,13 +1281,13 @@
         <v>90</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1288,13 +1301,13 @@
         <v>91</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1308,13 +1321,13 @@
         <v>92</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1328,13 +1341,13 @@
         <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1348,13 +1361,13 @@
         <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1368,13 +1381,13 @@
         <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1388,13 +1401,13 @@
         <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1408,13 +1421,13 @@
         <v>97</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1428,13 +1441,13 @@
         <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1448,13 +1461,13 @@
         <v>102</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F37" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1468,13 +1481,13 @@
         <v>104</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F38" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1488,13 +1501,13 @@
         <v>105</v>
       </c>
       <c r="E39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F39" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1508,13 +1521,13 @@
         <v>106</v>
       </c>
       <c r="E40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F40" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1528,13 +1541,13 @@
         <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F41" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1548,13 +1561,13 @@
         <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F42" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1568,13 +1581,13 @@
         <v>111</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1588,13 +1601,13 @@
         <v>112</v>
       </c>
       <c r="E44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1608,13 +1621,13 @@
         <v>113</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -1628,13 +1641,13 @@
         <v>117</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F46" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -1648,13 +1661,13 @@
         <v>127</v>
       </c>
       <c r="E47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -1668,13 +1681,13 @@
         <v>137</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -1688,13 +1701,13 @@
         <v>147</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1708,13 +1721,13 @@
         <v>151</v>
       </c>
       <c r="E50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F50" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -1728,13 +1741,13 @@
         <v>161</v>
       </c>
       <c r="E51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F51" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -1748,13 +1761,13 @@
         <v>166</v>
       </c>
       <c r="E52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -1768,13 +1781,13 @@
         <v>167</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F53" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -1788,13 +1801,13 @@
         <v>209</v>
       </c>
       <c r="E54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1808,10 +1821,10 @@
         <v>219</v>
       </c>
       <c r="E55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1838,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1837,7 +1850,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>